<commit_message>
updated mid-Atlantic study inputs
</commit_message>
<xml_diff>
--- a/projects/mid_atlantic/bct_monte_carlo/user_inputs_general.xlsx
+++ b/projects/mid_atlantic/bct_monte_carlo/user_inputs_general.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8758D6-BEA6-4344-932E-54B2AEA246B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B2C7FF-9644-41D7-8F35-4AA1BC6CED6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1115,7 +1115,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>